<commit_message>
Update IP - EX 37 - Validacao de dados (Anexo).xlsx
Formula add.
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 37 - Validacao de dados (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 37 - Validacao de dados (Anexo).xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F600866-F378-4761-9BB4-3B5CCA997E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D705DB3-8A99-4F7A-9F71-BEC17B460E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
     <sheet name="EXPLICAÇÃO" sheetId="4" r:id="rId2"/>
     <sheet name="EXERCÍCIOS" sheetId="5" r:id="rId3"/>
-    <sheet name="EXERCÍCIOS (RESOLVIDO)" sheetId="7" state="hidden" r:id="rId4"/>
+    <sheet name="EXERCÍCIOS (RESOLVIDO)" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="69">
   <si>
     <t>INSIRA UM NÚMERO (1 A 100):</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>*solução oculta</t>
+  </si>
+  <si>
+    <t>Turno ADM</t>
   </si>
 </sst>
 </file>
@@ -781,7 +784,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -894,36 +897,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2001,9 +1974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Planilha1"/>
   <dimension ref="B1:Q14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -2188,10 +2162,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Planilha2"/>
   <dimension ref="B1:W41"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2323,17 +2298,23 @@
       <c r="D10" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="24"/>
+      <c r="E10" s="24">
+        <v>20</v>
+      </c>
       <c r="G10" s="40"/>
       <c r="J10" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="24"/>
+      <c r="K10" s="24">
+        <v>0.1</v>
+      </c>
       <c r="M10" s="40"/>
       <c r="O10" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="P10" s="26"/>
+      <c r="P10" s="26">
+        <v>0.75</v>
+      </c>
       <c r="W10" t="s">
         <v>55</v>
       </c>
@@ -2347,13 +2328,17 @@
       <c r="B12" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="82"/>
-      <c r="E12" s="83"/>
+      <c r="D12" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="73"/>
       <c r="G12" s="40"/>
       <c r="J12" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="K12" s="25"/>
+      <c r="K12" s="25">
+        <v>35153</v>
+      </c>
       <c r="W12" t="s">
         <v>57</v>
       </c>
@@ -2367,8 +2352,8 @@
       <c r="F14" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="G14" s="93"/>
-      <c r="H14" s="81"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="71"/>
       <c r="W14" t="s">
         <v>59</v>
       </c>
@@ -2382,25 +2367,25 @@
       <c r="B16" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="84"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="85"/>
-      <c r="I16" s="86"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="76"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="87"/>
-      <c r="G17" s="88"/>
-      <c r="H17" s="88"/>
-      <c r="I17" s="89"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="79"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F18" s="90"/>
-      <c r="G18" s="91"/>
-      <c r="H18" s="91"/>
-      <c r="I18" s="92"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="82"/>
     </row>
     <row r="19" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
@@ -2429,17 +2414,23 @@
       <c r="D22" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E22" s="24"/>
+      <c r="E22" s="24">
+        <v>100</v>
+      </c>
       <c r="G22" s="40"/>
       <c r="J22" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="K22" s="24"/>
+      <c r="K22" s="24">
+        <v>0.1</v>
+      </c>
       <c r="M22" s="40"/>
       <c r="O22" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="P22" s="26"/>
+      <c r="P22" s="26">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="23" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J23" s="11"/>
@@ -2449,13 +2440,17 @@
       <c r="C24" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="80"/>
-      <c r="E24" s="81"/>
+      <c r="D24" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="73"/>
       <c r="G24" s="40"/>
       <c r="J24" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="K24" s="24"/>
+      <c r="K24" s="25">
+        <v>35153</v>
+      </c>
     </row>
     <row r="25" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
@@ -2463,30 +2458,34 @@
       <c r="F26" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="G26" s="80"/>
-      <c r="H26" s="81"/>
+      <c r="G26" s="83" t="s">
+        <v>68</v>
+      </c>
+      <c r="H26" s="71"/>
     </row>
     <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="F28" s="71"/>
-      <c r="G28" s="72"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="73"/>
+      <c r="F28" s="74">
+        <v>1234567891</v>
+      </c>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="76"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F29" s="74"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="76"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="78"/>
+      <c r="I29" s="79"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F30" s="77"/>
-      <c r="G30" s="78"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="79"/>
+      <c r="F30" s="80"/>
+      <c r="G30" s="81"/>
+      <c r="H30" s="81"/>
+      <c r="I30" s="82"/>
     </row>
     <row r="31" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
@@ -2628,30 +2627,37 @@
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="D24:E24"/>
   </mergeCells>
-  <dataValidations xWindow="740" yWindow="347" count="7">
+  <dataValidations xWindow="740" yWindow="347" count="9">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERRO" error="VOCÊ ESCOLHEU UM NÚMERO FORA DO INTERVALO CORRETO" promptTitle="INSTRUÇÃO" prompt="DIGITE UM NÚMERO ENTRE: 0,1 E 0,9" sqref="K10" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERRO" error="VOCÊ ESCOLHEU UM NÚMERO FORA DO INTERVALO CORRETO" promptTitle="INSTRUÇÃO" prompt="DIGITE UM NÚMERO ENTRE: 0,1 E 0,9" sqref="K10 K22" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>0.1</formula1>
       <formula2>0.9</formula2>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERRO" error="BIXO, VOCÊ ESTÁ QUERENDO ME FERRAR???_x000a_OLHA O HORÁRIO QUE VC QUER MARCAR A REUNIÃO..._x000a_MUDA ISSO AI VAI..._x000a_ASS: ESTAGIÁRIO" sqref="P10" xr:uid="{00000000-0002-0000-0100-000002000000}">
-      <formula1>0.208333333333333</formula1>
-      <formula2>0.875</formula2>
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERRO" error="BIXO, VOCÊ ESTÁ QUERENDO ME FERRAR???_x000a_OLHA O HORÁRIO QUE VC QUER MARCAR A REUNIÃO..._x000a_MUDA ISSO AI VAI..._x000a_ASS: ESTAGIÁRIO" sqref="P10 P22" xr:uid="{00000000-0002-0000-0100-000002000000}">
+      <formula1>0.333333333333333</formula1>
+      <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="date" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TEM CERTEZA?" error="VOCÊ ESTÁ QUERENDO INSERIR UMA DATA ANTIGA. CONFIRA. " sqref="K12" xr:uid="{00000000-0002-0000-0100-000004000000}">
+    <dataValidation type="date" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="TEM CERTEZA?" error="VOCÊ ESTÁ QUERENDO INSERIR UMA DATA ANTIGA. CONFIRA. " sqref="K12 K24" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>29346</formula1>
     </dataValidation>
     <dataValidation type="textLength" errorStyle="information" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERRO" error="VOCÊ ESTÁ TENTANDO INSERIR MAIS DO QUE 15 CARACTÉRES. ISTO PODE DAR PROBLEMA NO SISTEMA ERP. TEM CERTEZA?" sqref="F16:I18" xr:uid="{00000000-0002-0000-0100-000005000000}">
       <formula1>15</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14:H14" xr:uid="{00000000-0002-0000-0100-000006000000}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14:H14 G26:H26" xr:uid="{00000000-0002-0000-0100-000006000000}">
       <formula1>D12="OUTROS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:E12" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:E12 D24:E24" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>$W$9:$W$15</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erro 404" error="Leia a descrição!" promptTitle="Insira um número inteiro" prompt="1 a 100" sqref="E22" xr:uid="{3D29386E-62A4-4352-8E01-5379B0B443A5}">
+      <formula1>1</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERRO" error="VOCÊ ESTÁ TENTANDO INSERIR MAIS DO QUE 10 CARACTÉRES. ISTO PODE DAR PROBLEMA NO SISTEMA ERP. TEM CERTEZA?" sqref="F28:I30" xr:uid="{BEA72423-9C5C-4C38-9183-7BE2E85ECAD5}">
+      <formula1>10</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2661,13 +2667,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Planilha3"/>
   <dimension ref="B1:R35"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2808,10 +2818,10 @@
       <c r="B12" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="95" t="s">
+      <c r="D12" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="96"/>
+      <c r="E12" s="86"/>
       <c r="N12" s="5"/>
       <c r="Q12" s="6"/>
     </row>
@@ -2823,8 +2833,10 @@
       <c r="B14" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="95"/>
-      <c r="F14" s="96"/>
+      <c r="E14" s="85" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="86"/>
       <c r="N14" s="5"/>
       <c r="Q14" s="6"/>
     </row>
@@ -2838,12 +2850,16 @@
       <c r="B16" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="95"/>
-      <c r="F16" s="96"/>
+      <c r="E16" s="85">
+        <v>123456789</v>
+      </c>
+      <c r="F16" s="86"/>
       <c r="H16" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="45"/>
+      <c r="I16" s="45">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
@@ -2869,7 +2885,7 @@
         <v>100</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="L18" s="46">
         <f>(F18*H18*J18)/10^6</f>
@@ -2883,16 +2899,32 @@
       <c r="B20" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="97" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="97"/>
-      <c r="F20" s="97"/>
-      <c r="G20" s="97"/>
-      <c r="H20" s="97"/>
-      <c r="I20" s="97"/>
-      <c r="J20" s="97"/>
-      <c r="K20" s="97"/>
+      <c r="D20" s="87" t="str">
+        <f>IF(
+   OR(
+      L18&gt;1.4,
+      I16&gt;22,
+      ISBLANK(D12),
+      ISBLANK(E16),
+      ISBLANK(I16),
+      NOT(OR(D12="BRASIL",D12="ARGENTINA",D12="MÉXICO",D12="PERU",D12="CHILE")),
+      AND(D12="BRASIL",NOT(OR(E14="SP",E14="ITU",E14="SOROCABA"))),
+      AND(D12="ARGENTINA",NOT(OR(E14="BA",E14="SRL"))),
+      AND(OR(D12="MÉXICO",D12="PERU",D12="CHILE"),NOT(ISBLANK(E14))),
+      LEN(E16)&lt;&gt;9
+   ),
+   "NÃO LIBERADO",
+   "LIBERADO"
+)</f>
+        <v>LIBERADO</v>
+      </c>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="87"/>
+      <c r="K20" s="87"/>
     </row>
     <row r="23" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="51" t="s">
@@ -3023,16 +3055,16 @@
       <c r="B32" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="97" t="s">
+      <c r="D32" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="97"/>
-      <c r="F32" s="97"/>
-      <c r="G32" s="97"/>
-      <c r="H32" s="97"/>
-      <c r="I32" s="97"/>
-      <c r="J32" s="97"/>
-      <c r="K32" s="97"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="87"/>
+      <c r="I32" s="87"/>
+      <c r="J32" s="87"/>
+      <c r="K32" s="87"/>
       <c r="M32" t="s">
         <v>43</v>
       </c>
@@ -3046,16 +3078,16 @@
       <c r="B34" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="94" t="s">
+      <c r="D34" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="94"/>
-      <c r="F34" s="94"/>
-      <c r="G34" s="94"/>
-      <c r="H34" s="94"/>
-      <c r="I34" s="94"/>
-      <c r="J34" s="94"/>
-      <c r="K34" s="94"/>
+      <c r="E34" s="84"/>
+      <c r="F34" s="84"/>
+      <c r="G34" s="84"/>
+      <c r="H34" s="84"/>
+      <c r="I34" s="84"/>
+      <c r="J34" s="84"/>
+      <c r="K34" s="84"/>
       <c r="M34" t="s">
         <v>44</v>
       </c>
@@ -3090,6 +3122,24 @@
     <mergeCell ref="D20:K20"/>
     <mergeCell ref="D32:K32"/>
   </mergeCells>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:E12" xr:uid="{141A583C-1352-4900-8C2A-D46C698C6EA1}">
+      <formula1>$B$26:$B$30</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E14:F14" xr:uid="{C43414EE-48C8-410D-B915-C264307A17C9}">
+      <formula1>IF($D$12="BRASIL",$D$26:$D$28,IF($D$12="ARGENTINA",$G$26:$G$27,""))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Erro de preenchimento" error="O código da amostra deve ter 9 dígitos numéricos" sqref="E16:F16" xr:uid="{72F23E78-81B2-42B3-9198-AA703E15831B}">
+      <formula1>AND(LEN(E16)=9,ISNUMBER(E16))</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I16" xr:uid="{0EFD2E4A-244F-41EB-9A22-A3E688FEE468}">
+      <formula1>0.01</formula1>
+      <formula2>22</formula2>
+    </dataValidation>
+    <dataValidation type="custom" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L18" xr:uid="{7060E10D-5611-4897-BB78-095CF934F35F}">
+      <formula1>($F$18*$H$18*$J$18)&lt;=1400000</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3097,6 +3147,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7401CA-8A65-4EEB-B2A4-CC46B6D984EB}">
+  <sheetPr codeName="Planilha4"/>
   <dimension ref="B1:R35"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3239,10 +3290,10 @@
       <c r="B12" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="95" t="s">
+      <c r="D12" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="96"/>
+      <c r="E12" s="86"/>
       <c r="N12" s="5"/>
       <c r="Q12" s="6"/>
     </row>
@@ -3254,8 +3305,8 @@
       <c r="B14" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="95"/>
-      <c r="F14" s="96"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="86"/>
       <c r="N14" s="5"/>
       <c r="Q14" s="6"/>
     </row>
@@ -3269,10 +3320,10 @@
       <c r="B16" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="95">
+      <c r="E16" s="85">
         <v>667393221</v>
       </c>
-      <c r="F16" s="96"/>
+      <c r="F16" s="86"/>
       <c r="H16" s="52" t="s">
         <v>14</v>
       </c>
@@ -3318,17 +3369,17 @@
       <c r="B20" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="98" t="str">
+      <c r="D20" s="88" t="str">
         <f>IF(OR(D12="BRASIL",D12="ARGENTINA"),IF(AND(D12&lt;&gt;"",E14&lt;&gt;"",E16&lt;&gt;"",I16&lt;&gt;"",F18&lt;&gt;"",H18&lt;&gt;"",J18&lt;&gt;"",L18&lt;=1.4)=TRUE,"LIBERADO","NÃO LIBERADO"),IF(AND(D12&lt;&gt;"",E16&lt;&gt;"",I16&lt;&gt;"",F18&lt;&gt;"",H18&lt;&gt;"",J18&lt;&gt;"",L18&lt;=1.4)=TRUE,"LIBERADO","NÃO LIBERADO"))</f>
         <v>LIBERADO</v>
       </c>
-      <c r="E20" s="98"/>
-      <c r="F20" s="98"/>
-      <c r="G20" s="98"/>
-      <c r="H20" s="98"/>
-      <c r="I20" s="98"/>
-      <c r="J20" s="98"/>
-      <c r="K20" s="98"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="88"/>
+      <c r="J20" s="88"/>
+      <c r="K20" s="88"/>
       <c r="N20" s="54"/>
     </row>
     <row r="23" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -3460,16 +3511,16 @@
       <c r="B32" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="97" t="s">
+      <c r="D32" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="97"/>
-      <c r="F32" s="97"/>
-      <c r="G32" s="97"/>
-      <c r="H32" s="97"/>
-      <c r="I32" s="97"/>
-      <c r="J32" s="97"/>
-      <c r="K32" s="97"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="87"/>
+      <c r="I32" s="87"/>
+      <c r="J32" s="87"/>
+      <c r="K32" s="87"/>
       <c r="M32" t="s">
         <v>43</v>
       </c>
@@ -3483,16 +3534,16 @@
       <c r="B34" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="94" t="s">
+      <c r="D34" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="94"/>
-      <c r="F34" s="94"/>
-      <c r="G34" s="94"/>
-      <c r="H34" s="94"/>
-      <c r="I34" s="94"/>
-      <c r="J34" s="94"/>
-      <c r="K34" s="94"/>
+      <c r="E34" s="84"/>
+      <c r="F34" s="84"/>
+      <c r="G34" s="84"/>
+      <c r="H34" s="84"/>
+      <c r="I34" s="84"/>
+      <c r="J34" s="84"/>
+      <c r="K34" s="84"/>
       <c r="M34" t="s">
         <v>44</v>
       </c>

</xml_diff>